<commit_message>
Add data entry spreadsheet for PANELS
</commit_message>
<xml_diff>
--- a/sampling_event/final_spreadsheets/Sampling_Event_Protocol_marinegeo_protocol.xlsx
+++ b/sampling_event/final_spreadsheets/Sampling_Event_Protocol_marinegeo_protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\sampling_event\final_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4729E2CE-9D48-47DE-B0A8-3AE8CE0DE74A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C1D040-EE97-4ECF-BE61-92D701F99204}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="79">
   <si>
     <t>definition</t>
   </si>
@@ -72,9 +72,6 @@
     <t>field name</t>
   </si>
   <si>
-    <t>SAMPLING EVENT PROTOCOL</t>
-  </si>
-  <si>
     <t>camera_used</t>
   </si>
   <si>
@@ -117,6 +114,18 @@
     <t>The transect's minimum depth in meters.</t>
   </si>
   <si>
+    <t>dissolved_oxygen</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen measured by a sonde or probe</t>
+  </si>
+  <si>
+    <t>dissolved_oxygen_unit</t>
+  </si>
+  <si>
+    <t>Unit associated with dissolved oxygen</t>
+  </si>
+  <si>
     <t>habitat_type</t>
   </si>
   <si>
@@ -150,9 +159,6 @@
     <t>The direction of the camera when the image is captured, in degrees (0-359)</t>
   </si>
   <si>
-    <t>degrees</t>
-  </si>
-  <si>
     <t>photo_filename</t>
   </si>
   <si>
@@ -171,6 +177,12 @@
     <t>Person who captured the site photograph</t>
   </si>
   <si>
+    <t>salinity_ppt</t>
+  </si>
+  <si>
+    <t>Salinity, measured with a probe, sonde, or refractometer, in parts per thousand</t>
+  </si>
+  <si>
     <t>sample_collection_day</t>
   </si>
   <si>
@@ -219,6 +231,12 @@
     <t>Any additional notes regarding observations, context, or concerns about the site location</t>
   </si>
   <si>
+    <t>temperature_c</t>
+  </si>
+  <si>
+    <t>Temperature, measured with a probe or sonde, in degrees Celsius</t>
+  </si>
+  <si>
     <t>transect</t>
   </si>
   <si>
@@ -262,6 +280,9 @@
   </si>
   <si>
     <t>Site visibility in meters</t>
+  </si>
+  <si>
+    <t>SAMPLING EVENT &amp; ENVIRONMENTAL MONITORING PROTOCOL</t>
   </si>
 </sst>
 </file>
@@ -416,6 +437,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -439,9 +463,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -822,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,30 +859,30 @@
     <col min="6" max="6" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3"/>
-      <c r="B1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="7" t="s">
+    <row r="1" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="4"/>
+      <c r="B1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:7" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -885,432 +906,494 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="F32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1329,14 +1412,14 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1348,56 +1431,72 @@
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" customWidth="1"/>
+    <col min="13" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="6" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>55</v>
+      <c r="R1" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1425,29 +1524,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="A1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>28</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1479,44 +1578,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="A1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>68</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>